<commit_message>
updated initial phase graph
</commit_message>
<xml_diff>
--- a/Medication Timing Estimated Graphs.xlsx
+++ b/Medication Timing Estimated Graphs.xlsx
@@ -216,12 +216,12 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$27:$A$46</c:f>
+              <c:f>Sheet1!$A$27:$A$31</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$46</c:f>
+              <c:f>Sheet1!$B$27:$B$31</c:f>
               <c:numCache/>
             </c:numRef>
           </c:yVal>
@@ -234,11 +234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1199638571"/>
-        <c:axId val="363516092"/>
+        <c:axId val="2016208008"/>
+        <c:axId val="151439582"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1199638571"/>
+        <c:axId val="2016208008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,10 +313,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363516092"/>
+        <c:crossAx val="151439582"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363516092"/>
+        <c:axId val="151439582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +391,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1199638571"/>
+        <c:crossAx val="2016208008"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -500,11 +500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1690991110"/>
-        <c:axId val="240005118"/>
+        <c:axId val="1347134502"/>
+        <c:axId val="468992927"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1690991110"/>
+        <c:axId val="1347134502"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,10 +579,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240005118"/>
+        <c:crossAx val="468992927"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240005118"/>
+        <c:axId val="468992927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1690991110"/>
+        <c:crossAx val="1347134502"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -779,11 +779,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1390753586"/>
-        <c:axId val="1801830651"/>
+        <c:axId val="1604940447"/>
+        <c:axId val="91792407"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1390753586"/>
+        <c:axId val="1604940447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,10 +858,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1801830651"/>
+        <c:crossAx val="91792407"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1801830651"/>
+        <c:axId val="91792407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +936,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1390753586"/>
+        <c:crossAx val="1604940447"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1058,11 +1058,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="732310028"/>
-        <c:axId val="1439047364"/>
+        <c:axId val="760233338"/>
+        <c:axId val="2065039112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="732310028"/>
+        <c:axId val="760233338"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,10 +1137,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1439047364"/>
+        <c:crossAx val="2065039112"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1439047364"/>
+        <c:axId val="2065039112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1215,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="732310028"/>
+        <c:crossAx val="760233338"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>